<commit_message>
Updated to show Power
</commit_message>
<xml_diff>
--- a/Code/PythonCode/Python1/Working/sensor_data7cm_4hz_third.xlsx
+++ b/Code/PythonCode/Python1/Working/sensor_data7cm_4hz_third.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,90 +441,104 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Temp</t>
+          <t>Temp (°C)</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Voltage</t>
+          <t>Voltage (V)</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Current</t>
+          <t>Current (mA)</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Elapsed Time</t>
+          <t>Power (W)</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Elapsed Time (s)</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>0d0h13m3</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>23.8</v>
+        <v>23.9</v>
       </c>
       <c r="C2" t="n">
-        <v>1.73</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>0.8632190227508545</v>
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.5986261367797852</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>0d0h13m3</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>23.7</v>
+        <v>24</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>2.374584436416626</v>
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2.105473279953003</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>0d0h13m3</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="C4" t="n">
-        <v>1.61</v>
+        <v>0</v>
       </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>3.878249406814575</v>
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>3.608244657516479</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>0d0h13m3</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
@@ -533,150 +547,174 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>6.921084403991699</v>
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>5.115900754928589</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>0d0h13m3</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="C6" t="n">
-        <v>1.39</v>
+        <v>0</v>
       </c>
       <c r="D6" t="n">
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>8.428021430969238</v>
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>6.618702411651611</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>0d0h13m4</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>23.8</v>
+        <v>23.9</v>
       </c>
       <c r="C7" t="n">
-        <v>1.1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>9.939008712768555</v>
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>8.126445770263672</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>0d0h13m4</t>
+          <t>0d0h31m5</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>23.8</v>
+        <v>24.1</v>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>0.42</v>
       </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>11.45068025588989</v>
+        <v>9.799999999999998e-05</v>
+      </c>
+      <c r="F8" t="n">
+        <v>9.629774332046509</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>0d0h13m4</t>
+          <t>0d0h32m0</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>23.8</v>
+        <v>23.9</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="E9" t="n">
-        <v>12.95792365074158</v>
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>11.13293600082397</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>0d0h13m4</t>
+          <t>0d0h32m2</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>23.8</v>
+        <v>24.1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D10" t="n">
-        <v>0.02</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>14.46582889556885</v>
+        <v>0.0001742222222222223</v>
+      </c>
+      <c r="F10" t="n">
+        <v>12.63974785804749</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>0d0h13m4</t>
+          <t>0d0h32m3</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>23.8</v>
+        <v>23.9</v>
       </c>
       <c r="C11" t="n">
-        <v>0.29</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E11" t="n">
-        <v>15.96834230422974</v>
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>14.14341926574707</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>0d0h13m4</t>
+          <t>0d0h32m5</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>23.7</v>
+        <v>24</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>0.02</v>
+        <v>0.01</v>
       </c>
       <c r="E12" t="n">
-        <v>17.47588157653809</v>
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>15.6506404876709</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>0d0h13m5</t>
+          <t>0d0h32m6</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -685,17 +723,20 @@
         <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>18.98284602165222</v>
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>17.15355730056763</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>0d0h13m5</t>
+          <t>0d0h32m8</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>23.8</v>
+        <v>24.1</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
@@ -704,17 +745,20 @@
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>20.49046015739441</v>
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>18.65697908401489</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>0d0h13m5</t>
+          <t>0d0h32m9</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
@@ -723,64 +767,406 @@
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>21.9979419708252</v>
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>20.15951108932495</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>0d0h13m5</t>
+          <t>0d0h32m1</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23.8</v>
+        <v>24.1</v>
       </c>
       <c r="C16" t="n">
-        <v>0</v>
+        <v>1.51</v>
       </c>
       <c r="D16" t="n">
         <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>23.504314661026</v>
+        <v>0.001266722222222222</v>
+      </c>
+      <c r="F16" t="n">
+        <v>21.66722917556763</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>0d0h13m5</t>
+          <t>0d0h32m1</t>
         </is>
       </c>
       <c r="B17" t="n">
         <v>23.8</v>
       </c>
       <c r="C17" t="n">
-        <v>0</v>
+        <v>0.71</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>26.55250334739685</v>
+        <v>0.0002800555555555555</v>
+      </c>
+      <c r="F17" t="n">
+        <v>23.1697199344635</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>0d0h14m0</t>
+          <t>0d0h32m1</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>23.8</v>
+        <v>24</v>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>1.64</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>29.59527683258057</v>
+        <v>0.001494222222222222</v>
+      </c>
+      <c r="F18" t="n">
+        <v>24.67335438728333</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>0d0h32m1</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>24</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>26.18044018745422</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>0d0h32m1</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>27.6843421459198</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>0d0h32m1</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
+      <c r="F21" t="n">
+        <v>29.19188261032104</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
+      <c r="F22" t="n">
+        <v>30.69759321212769</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>24</v>
+      </c>
+      <c r="C23" t="n">
+        <v>3.08</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0.005270222222222222</v>
+      </c>
+      <c r="F23" t="n">
+        <v>32.20168089866638</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>33.70922541618347</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>35.21572542190552</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.78</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0.000338</v>
+      </c>
+      <c r="F26" t="n">
+        <v>36.71937704086304</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>38.23027110099792</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>0d0h32m2</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>39.73340916633606</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>0d0h32m3</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>41.23675870895386</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>0d0h32m3</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>42.74416780471802</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>0d0h32m3</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>44.24688673019409</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>0d0h32m3</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>23.9</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>45.75023293495178</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>0d0h32m3</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>24</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>47.25340867042542</v>
       </c>
     </row>
   </sheetData>

</xml_diff>